<commit_message>
latency of 100ms works at 80mph. still flaky. need to find better parameters. and clean up the code
</commit_message>
<xml_diff>
--- a/motion-analysis.xlsx
+++ b/motion-analysis.xlsx
@@ -16,36 +16,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>dt</t>
-  </si>
-  <si>
-    <t>dv</t>
-  </si>
-  <si>
-    <t>px</t>
-  </si>
-  <si>
-    <t>py</t>
-  </si>
-  <si>
-    <t>move</t>
-  </si>
-  <si>
-    <t>pred move</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>dv/dt, m/s2</t>
   </si>
   <si>
-    <t>dv/dt</t>
+    <t>px, un</t>
+  </si>
+  <si>
+    <t>v, mph</t>
+  </si>
+  <si>
+    <t>py, un</t>
+  </si>
+  <si>
+    <t>move, un</t>
+  </si>
+  <si>
+    <t>dt, sec</t>
+  </si>
+  <si>
+    <t>t, sec</t>
+  </si>
+  <si>
+    <t>move/dt, un/s</t>
+  </si>
+  <si>
+    <t>v, m/s</t>
+  </si>
+  <si>
+    <t>dv, m/s</t>
+  </si>
+  <si>
+    <t>pred move, m</t>
   </si>
 </sst>
 </file>
@@ -377,50 +380,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K6"/>
+  <dimension ref="B1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:12">
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
+      <c r="L1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:12">
       <c r="B2">
         <v>0.68902200000000002</v>
       </c>
@@ -433,8 +442,12 @@
       <c r="E2">
         <v>108.51</v>
       </c>
+      <c r="I2">
+        <f>C2*1609/3600</f>
+        <v>1.3489006805555555</v>
+      </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:12">
       <c r="B3">
         <v>0.79597399999999996</v>
       </c>
@@ -456,23 +469,27 @@
         <v>0.10695199999999994</v>
       </c>
       <c r="H3">
-        <f>C3-C2</f>
-        <v>0.92660000000000009</v>
+        <f>F3/G3</f>
+        <v>1.7779942204245913</v>
       </c>
       <c r="I3">
-        <f>H3/G3</f>
-        <v>8.663699603560481</v>
+        <f t="shared" ref="I3:I6" si="0">C3*1609/3600</f>
+        <v>1.7630394027777778</v>
       </c>
       <c r="J3">
-        <f>(H3/G3)*(1609/3600)</f>
-        <v>3.8721924061468926</v>
+        <f>I3-I2</f>
+        <v>0.41413872222222237</v>
       </c>
       <c r="K3">
-        <f>C2*(B3-B2)+I3/2*(B3-B2)^2</f>
-        <v>0.37233734519999984</v>
+        <f>J3/G3</f>
+        <v>3.872192406146894</v>
+      </c>
+      <c r="L3">
+        <f>I2*G3+K3/2*G3^2</f>
+        <v>0.16641410789633324</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:12">
       <c r="B4">
         <v>0.93561099999999997</v>
       </c>
@@ -486,7 +503,7 @@
         <v>108.211</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F6" si="0">SQRT((D4-D3)^2+(E4-E3)^2)</f>
+        <f t="shared" ref="F4:F6" si="1">SQRT((D4-D3)^2+(E4-E3)^2)</f>
         <v>0.33975298379852537</v>
       </c>
       <c r="G4">
@@ -494,23 +511,27 @@
         <v>0.13963700000000001</v>
       </c>
       <c r="H4">
-        <f>C4-C3</f>
-        <v>1.4675099999999999</v>
+        <f t="shared" ref="H4:H6" si="2">F4/G4</f>
+        <v>2.4331157486806889</v>
       </c>
       <c r="I4">
-        <f>H4/G4</f>
-        <v>10.509463824058091</v>
+        <f t="shared" si="0"/>
+        <v>2.4189348444444447</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J6" si="1">(H4/G4)*(1609/3600)</f>
-        <v>4.6971464702526298</v>
+        <f t="shared" ref="J4:J6" si="3">I4-I3</f>
+        <v>0.65589544166666691</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K6" si="2">C3*(B4-B3)+I4/2*(B4-B3)^2</f>
-        <v>0.65327843898500015</v>
+        <f t="shared" ref="K4:K6" si="4">J4/G4</f>
+        <v>4.6971464702526324</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L6" si="5">I3*G4+K4/2*G4^2</f>
+        <v>0.29197916897968479</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:12">
       <c r="B5">
         <v>1.1363399999999999</v>
       </c>
@@ -524,7 +545,7 @@
         <v>107.83799999999999</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.65984201897121042</v>
       </c>
       <c r="G5">
@@ -532,23 +553,27 @@
         <v>0.20072899999999994</v>
       </c>
       <c r="H5">
-        <f>C5-C4</f>
-        <v>2.4246299999999996</v>
+        <f t="shared" si="2"/>
+        <v>3.2872281482556613</v>
       </c>
       <c r="I5">
-        <f>H5/G5</f>
-        <v>12.079121601761582</v>
+        <f t="shared" si="0"/>
+        <v>3.5026097527777775</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
-        <v>5.3986962936762177</v>
+        <f t="shared" si="3"/>
+        <v>1.0836749083333328</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
-        <v>1.3297242422749997</v>
+        <f t="shared" si="4"/>
+        <v>5.398696293676216</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="5"/>
+        <v>0.59431286272790951</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:12">
       <c r="B6">
         <v>2.19739</v>
       </c>
@@ -562,7 +587,7 @@
         <v>103.69499999999999</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.2065484498475412</v>
       </c>
       <c r="G6">
@@ -570,20 +595,24 @@
         <v>1.06105</v>
       </c>
       <c r="H6">
-        <f>C6-C5</f>
-        <v>12.24671</v>
+        <f t="shared" si="2"/>
+        <v>6.7919027848334581</v>
       </c>
       <c r="I6">
-        <f>H6/G6</f>
-        <v>11.542066820602233</v>
+        <f t="shared" si="0"/>
+        <v>8.9762087499999996</v>
       </c>
       <c r="J6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>5.4735989972222221</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
         <v>5.1586626428747202</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="2"/>
-        <v>14.812411852250001</v>
+      <c r="L6">
+        <f t="shared" si="5"/>
+        <v>6.6203251861861805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>